<commit_message>
Feat: Agrega validacion en funciones
</commit_message>
<xml_diff>
--- a/data/parametros/Equivalencias.xlsx
+++ b/data/parametros/Equivalencias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\cod\dev\journals-amalia\data\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE24650D-BD20-457D-9630-83D4ADE433FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A8D98A-BA07-4C05-9B64-7176014779B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F14BC482-54BA-4309-9DDB-9067717A7710}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F14BC482-54BA-4309-9DDB-9067717A7710}"/>
   </bookViews>
   <sheets>
     <sheet name="Parametros" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="125">
   <si>
     <t>id netsuite</t>
   </si>
@@ -365,6 +365,54 @@
   </si>
   <si>
     <t>ID_TERCERO</t>
+  </si>
+  <si>
+    <t>COLPENSIONES 900336004</t>
+  </si>
+  <si>
+    <t>EPS SERVICIO OCCIDENTAL DE SALUD SA</t>
+  </si>
+  <si>
+    <t>SENA - PARAFISCALES</t>
+  </si>
+  <si>
+    <t>SENA 899999034</t>
+  </si>
+  <si>
+    <t>ICBF 899999239</t>
+  </si>
+  <si>
+    <t>ICBF - PARAFISCALES</t>
+  </si>
+  <si>
+    <t>CAJA DE COMPENSACION FAMILIAR DE CORDOBA COMFACOR 891080005</t>
+  </si>
+  <si>
+    <t>COMFACOR - CAJA DE COMPENSACIÓN</t>
+  </si>
+  <si>
+    <t>COLFONDOS - PENSIÓN</t>
+  </si>
+  <si>
+    <t>COMFAMILIAR ANDI COMFANDI</t>
+  </si>
+  <si>
+    <t>COMFANDI - CAJA DE COMPENSACIÓN</t>
+  </si>
+  <si>
+    <t>CAJA COLOMBIANA DE SUBSIDIO FAMILIAR COLSUBSIDIO</t>
+  </si>
+  <si>
+    <t>COLSUBSIDIO - CAJA DE COMPENSACIÓN</t>
+  </si>
+  <si>
+    <t>AXA COLPATRIA SEGUROS DE VIDA SA</t>
+  </si>
+  <si>
+    <t>AXA COLPATRIA ARL - APORTES A ADMINISTRADORAS DE RIESGOS PROFESIONALES</t>
+  </si>
+  <si>
+    <t>COLPENSIONES - PENSIÓN</t>
   </si>
 </sst>
 </file>
@@ -766,7 +814,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,15 +867,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523C8900-6C0A-4C12-AB61-48A5E72FB227}">
-  <dimension ref="A1:E55"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
@@ -1574,6 +1623,15 @@
       <c r="B45" s="1">
         <v>900336004</v>
       </c>
+      <c r="C45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45">
+        <v>149463</v>
+      </c>
+      <c r="E45" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1626,12 +1684,21 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B49" s="1">
         <v>805001157</v>
+      </c>
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49">
+        <v>149681</v>
+      </c>
+      <c r="E49" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1733,6 +1800,142 @@
         <v>149473</v>
       </c>
       <c r="E55" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" s="1">
+        <v>899999034</v>
+      </c>
+      <c r="C56" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56">
+        <v>149465</v>
+      </c>
+      <c r="E56" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" s="1">
+        <v>899999239</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="1">
+        <v>149467</v>
+      </c>
+      <c r="E57" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="1">
+        <v>891080005</v>
+      </c>
+      <c r="C58" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58">
+        <v>149680</v>
+      </c>
+      <c r="E58" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="1">
+        <v>800227940</v>
+      </c>
+      <c r="C59" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59">
+        <v>149471</v>
+      </c>
+      <c r="E59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" s="1">
+        <v>890303208</v>
+      </c>
+      <c r="C60" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60">
+        <v>5917</v>
+      </c>
+      <c r="E60" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" s="1">
+        <v>860007336</v>
+      </c>
+      <c r="C61" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61">
+        <v>149679</v>
+      </c>
+      <c r="E61" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" s="1">
+        <v>860002183</v>
+      </c>
+      <c r="C62" t="s">
+        <v>122</v>
+      </c>
+      <c r="D62">
+        <v>149678</v>
+      </c>
+      <c r="E62" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="1">
+        <v>900336004</v>
+      </c>
+      <c r="C63" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63">
+        <v>149463</v>
+      </c>
+      <c r="E63" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>